<commit_message>
Updated Testcases for expected db value checks
</commit_message>
<xml_diff>
--- a/test_data/film_test_data.xlsx
+++ b/test_data/film_test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\driver\PythonProject\PythonProject\api-framework\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\driver\api-framework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55C8A7C-806D-4062-9E50-94463472D89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2277126B-4FEC-490E-B870-1BF6658FAF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>title</t>
   </si>
@@ -59,116 +59,89 @@
     <t>expected_response</t>
   </si>
   <si>
-    <t>film_id</t>
-  </si>
-  <si>
     <t>Trailers , Deleted Scenes</t>
   </si>
   <si>
     <t>adapt:1 , astound:4 ,baloon:19 , car:11 , factori :20</t>
   </si>
   <si>
+    <t>PG-13</t>
+  </si>
+  <si>
+    <t>Die Hard</t>
+  </si>
+  <si>
+    <t>Terminator</t>
+  </si>
+  <si>
+    <t>12 angry man</t>
+  </si>
+  <si>
+    <t>The Shawshank redemption</t>
+  </si>
+  <si>
+    <t>A cyborg assassin is sent back in time from a dystopian future (2029) to 1984 Los Angeles to kill Sarah Connor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banker Andy Dufresne is wrongfully convicted of the murders of his wife and her lover and sentenced to life imprisonment at the brutal Shawshank State Penitentiary. </t>
+  </si>
+  <si>
+    <t>New York City Police detective John McClane  arrives in Los Angeles on Christmas Eve to reconcile with his estranged wife at her company's holiday party.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> {
-    "film_id": 3013,
-    "title": "The Godfather",
-    "description": "Classic",
-    "release_year": 1975,
+    "title": "Terminator",
+    "description": "A cyborg assassin is sent back in time from a dystopian future (2029) to 1984 Los Angeles to kill Sarah Connor",
+    "release_year": 1984,
+    "language_id": 1,
+    "rental_duration": 1,
+    "rental_rate": 2.99,
+    "length": 204,
+    "replacement_cost": 2.99,
+    "rating": "PG-13"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {
+    "title": "12 angry man",
+    "description": "In a New York City courthouse on a sweltering hot day, a jury of twelve men must decide the fate of an inner-city teenager accused of murdering his father.",
+    "release_year": 1957,
     "language_id": 1,
     "rental_duration": 2,
     "rental_rate": 1.99,
     "length": 197,
     "replacement_cost": 1.99,
-    "rating": 9,
-    "special_features": [
-      "Trailers",
-      "Deleted Scenes"
-    ],
-    "fulltext": "'adapt':1 'astound':4 'baloon':19 'car':11 'factori':20 'hole':2 'lumberjack':8,16 'must':13 'reflect':5 'sink':14"
+    "rating": "PG-13"
 }</t>
   </si>
   <si>
     <t xml:space="preserve"> {
-    "film_id": 3013,
-    "title": "The Godfather 2",
-    "description": "Classic",
-    "release_year": 1980,
+    "title": "The Shawshank redemption",
+    "description": "Banker Andy Dufresne is wrongfully convicted of the murders of his wife and her lover and sentenced to life imprisonment at the brutal Shawshank State Penitentiary. ",
+    "release_year": 1994,
     "language_id": 1,
-    "rental_duration": 2,
-    "rental_rate": 1.99,
-    "length": 197,
-    "replacement_cost": 1.99,
-    "rating": 9,
-    "special_features": [
-      "Trailers",
-      "Deleted Scenes"
-    ],
-    "fulltext": "'adapt':1 'astound':4 'baloon':19 'car':11 'factori':20 'hole':2 'lumberjack':8,16 'must':13 'reflect':5 'sink':14"
+    "rental_duration": 3,
+    "rental_rate": 0.99,
+    "length": 125,
+    "replacement_cost": 0.99,
+    "rating": "PG-13"
 }</t>
   </si>
   <si>
     <t xml:space="preserve"> {
-    "film_id": 3015,
-    "title": "Mission Impossible",
-    "description": "Best action",
-    "release_year": 2002,
+    "title": "Die Hard",
+    "description": "New York City Police detective John McClane  arrives in Los Angeles on Christmas Eve to reconcile with his estranged wife at her company's holiday party.",
+    "release_year": 1988,
     "language_id": 1,
-    "rental_duration": 12,
+    "rental_duration": 4,
     "rental_rate": 2.99,
     "length": 170,
     "replacement_cost": 2.99,
-    "rating": 9,
-    "special_features": [
-      "Trailers",
-      "Deleted Scenes"
-    ],
-    "fulltext": "'adapt':1 'astound':4 'baloon':19 'car':11 'factori':20 'hole':2 'lumberjack':8,16 'must':13 'reflect':5 'sink':14"
+    "rating": "PG-13"
 }</t>
   </si>
   <si>
-    <t xml:space="preserve"> {
-    "film_id": 3012,
-    "title": "Matrix",
-    "description": "Sifi movie",
-    "release_year": 2002,
-    "language_id": 1,
-    "rental_duration": 1,
-    "rental_rate": 2.99,
-    "length": 204,
-    "replacement_cost": 2.99,
-    "rating": 9,
-    "special_features": [
-      "Trailers",
-      "Deleted Scenes"
-    ],
-    "fulltext": "'adapt':1 'astound':4 'baloon':19 'car':11 'factori':20 'hole':2 'lumberjack':8,16 'must':13 'reflect':5 'sink':14"
-}</t>
-  </si>
-  <si>
-    <t>PG-13</t>
-  </si>
-  <si>
-    <t>Die Hard</t>
-  </si>
-  <si>
-    <t>Terminator</t>
-  </si>
-  <si>
-    <t>12 angry man</t>
-  </si>
-  <si>
-    <t>The Shawshank redemption</t>
-  </si>
-  <si>
-    <t>A cyborg assassin (Arnold Schwarzenegger) is sent back in time from a dystopian future (2029) to 1984 Los Angeles to kill Sarah Connor (Linda Hamilton), the woman whose unborn son is destined to lead the human resistance against the machines (Skynet). A human soldier, Kyle Reese, is also sent back to protect her, leading to a relentless pursuit and a race against time.</t>
-  </si>
-  <si>
-    <t>In a New York City courthouse on a sweltering hot day, a jury of twelve men must decide the fate of an inner-city teenager accused of murdering his father. The case seems open-and-shut, with eleven jurors quickly voting "guilty." However, one juror (Henry Fonda) expresses "reasonable doubt," forcing the group to meticulously re-examine the evidence, confront their personal biases, and engage in a tense deliberation to reach a unanimous verdict.</t>
-  </si>
-  <si>
-    <t>Banker Andy Dufresne (Tim Robbins) is wrongfully convicted of the murders of his wife and her lover and sentenced to life imprisonment at the brutal Shawshank State Penitentiary. Over nearly two decades, he maintains his dignity, befriends fellow inmate Ellis "Red" Redding (Morgan Freeman), and uses his financial expertise to aid the corrupt warden's money-laundering operation, all while secretly planning an audacious escape driven by an unwavering sense of hope.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New York City Police detective John McClane (Bruce Willis) arrives in Los Angeles on Christmas Eve to reconcile with his estranged wife at her company's holiday party. The festivities are interrupted when a group of cunning thieves, posing as terrorists and led by the ruthless Hans Gruber (Alan Rickman), seize the skyscraper and take the attendees hostage. Trapped and largely on his own, a wisecracking McClane must battle the invaders floor by floor to save the hostages and his wife. </t>
+    <t>In a New York City courthouse on a sweltering hot day, a jury of twelve men must decide the fate of an inner-city teenager accused of murdering his father.</t>
   </si>
 </sst>
 </file>
@@ -523,229 +496,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="50" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="11" width="25" customWidth="1"/>
+    <col min="12" max="12" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1984</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2.99</v>
+      </c>
+      <c r="G2">
+        <v>204</v>
+      </c>
+      <c r="H2">
+        <v>2.99</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3012</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2">
-        <v>1984</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2.99</v>
-      </c>
-      <c r="H2">
-        <v>204</v>
-      </c>
-      <c r="I2">
-        <v>2.99</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
       </c>
       <c r="L2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>1957</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1.99</v>
+      </c>
+      <c r="G3">
+        <v>197</v>
+      </c>
+      <c r="H3">
+        <v>1.99</v>
+      </c>
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3013</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3">
-        <v>1957</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>1.99</v>
-      </c>
-      <c r="H3">
-        <v>197</v>
-      </c>
-      <c r="I3">
-        <v>1.99</v>
-      </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s">
         <v>13</v>
       </c>
       <c r="L3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>1994</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0.99</v>
+      </c>
+      <c r="G4">
+        <v>125</v>
+      </c>
+      <c r="H4">
+        <v>0.99</v>
+      </c>
+      <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="M3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3014</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4">
-        <v>1994</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>0.99</v>
-      </c>
-      <c r="H4">
-        <v>125</v>
-      </c>
-      <c r="I4">
-        <v>0.99</v>
-      </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
       </c>
       <c r="L4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>1988</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>2.99</v>
+      </c>
+      <c r="G5">
+        <v>170</v>
+      </c>
+      <c r="H5">
+        <v>2.99</v>
+      </c>
+      <c r="I5" t="s">
         <v>14</v>
       </c>
-      <c r="M4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3015</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5">
-        <v>1988</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>2.99</v>
-      </c>
-      <c r="H5">
-        <v>170</v>
-      </c>
-      <c r="I5">
-        <v>2.99</v>
-      </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +716,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,10 +764,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>1984</v>
@@ -830,15 +788,15 @@
         <v>2.99</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>1957</v>
@@ -859,15 +817,15 @@
         <v>1.99</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>1994</v>
@@ -888,15 +846,15 @@
         <v>0.99</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>1988</v>
@@ -917,7 +875,7 @@
         <v>2.99</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>